<commit_message>
DOC - 1/14 Femto 전달 문서
</commit_message>
<xml_diff>
--- a/0_DOC/Plasma_Gen_Q&A_list_20171127.xlsx
+++ b/0_DOC/Plasma_Gen_Q&A_list_20171127.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="1월12일 meeting" sheetId="4" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Plasma_Gen!$A$1:$H$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Plasma_LF!$A$1:$H$16</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -273,6 +273,17 @@
   </si>
   <si>
     <t>Main PCB P3, P4 CON에 연결되는 ADC와 GPIO 구현 여부</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>External Power model에서 불필요한 기능 확인
+ - 전원 Key, Plasma Key, Volume Key
+ - Buzzer
+ - 충전 IC, Battery, Battery CON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery model에서 RS-232 통신 지원 여부</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -692,6 +703,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -703,12 +720,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,7 +781,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -805,7 +816,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1016,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1041,7 +1052,7 @@
       <c r="B4" s="27"/>
     </row>
     <row r="5" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1052,7 +1063,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C6" s="29"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="8" t="s">
         <v>18</v>
       </c>
@@ -1061,7 +1072,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="C7" s="29"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="8" t="s">
         <v>19</v>
       </c>
@@ -1070,7 +1081,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="32" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -1081,11 +1092,11 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C9" s="31"/>
-      <c r="D9" s="32" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="29" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1305,7 +1316,7 @@
       <c r="G8" s="18"/>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>6</v>
       </c>
@@ -1429,14 +1440,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="66" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>12</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="C15" s="6">
+        <v>43114</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="G15" s="18"/>
       <c r="H15" s="23"/>
     </row>
@@ -1444,10 +1463,18 @@
       <c r="B16" s="5">
         <v>13</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="C16" s="6">
+        <v>43114</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="G16" s="18"/>
       <c r="H16" s="23"/>
     </row>
@@ -1627,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
DOC - Q&A list update
</commit_message>
<xml_diff>
--- a/0_DOC/Plasma_Gen_Q&A_list_20171127.xlsx
+++ b/0_DOC/Plasma_Gen_Q&A_list_20171127.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1월12일 meeting" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -284,6 +284,11 @@
   </si>
   <si>
     <t>Battery model에서 RS-232 통신 지원 여부</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>J9의 Pin-23,Pin-27에 연결된 Pull-up 저항의 역할 확인 필요함
+ LF main board에서 4.7K Pull-up 저항과 연결이되며, 이 두개의 Pin으로 확인을 하는 사항이 무엇인지 확인 필요함</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -781,7 +786,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -816,7 +821,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1027,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1177,7 +1182,7 @@
   <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1654,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1775,14 +1780,16 @@
       <c r="G7" s="17"/>
       <c r="H7" s="23"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>5</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="G8" s="18"/>
       <c r="H8" s="23"/>
     </row>

</xml_diff>